<commit_message>
Fixed on reports column order for Daily Detailed Transactions Report. Fixed Register new user account.
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/DailyDetailedTransactionsReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/DailyDetailedTransactionsReport_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B263D5E8-127E-4A41-B8AB-796168BBF4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B0E46B-FE4F-410A-9FAB-D83642990585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D669A5D4-6159-4454-8903-2CDEC1F5EAD7}"/>
   </bookViews>
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -126,6 +126,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +447,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M2:M8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +461,7 @@
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -490,7 +494,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">

</xml_diff>

<commit_message>
#197-Modified Daily Detailed Transactions Report
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/DailyDetailedTransactionsReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/DailyDetailedTransactionsReport_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B0E46B-FE4F-410A-9FAB-D83642990585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDEFBC0-D5C0-4697-843E-FC662ED80290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D669A5D4-6159-4454-8903-2CDEC1F5EAD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Store Name</t>
   </si>
@@ -74,7 +74,19 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Order Status</t>
+  </si>
+  <si>
+    <t>Paid Status</t>
+  </si>
+  <si>
+    <t>Return Items</t>
+  </si>
+  <si>
+    <t>Sales Agent</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -118,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -130,6 +142,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,9 +161,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -188,7 +201,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -294,7 +307,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165E5DC9-291D-4F77-BA6D-54A38C7460AD}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,49 +475,67 @@
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>